<commit_message>
Data fix for few Incorect URL's changed aftected by migration
</commit_message>
<xml_diff>
--- a/test-data/leadimage-data.xlsx
+++ b/test-data/leadimage-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/popkhadzeg/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45512A95-66D2-48FC-9B31-8E4EA781D466}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6019496-5710-E249-9EEE-A92F80194D5B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2760" windowWidth="14930" windowHeight="5460" firstSheet="2" activeTab="4" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="1760" yWindow="1780" windowWidth="32020" windowHeight="14940" firstSheet="3" activeTab="3" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_leadimage" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="48">
   <si>
     <t>path</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>patients with chronic leukemia</t>
+  </si>
+  <si>
+    <t>Crédito: Instituto Nacional del Cáncer</t>
   </si>
 </sst>
 </file>
@@ -530,14 +533,14 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -577,7 +580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -597,7 +600,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -617,7 +620,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -637,7 +640,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -670,14 +673,14 @@
       <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -699,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -710,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -721,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -732,7 +735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -743,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -767,15 +770,15 @@
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="66.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -795,7 +798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -815,7 +818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -835,7 +838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -852,7 +855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -869,7 +872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -886,7 +889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -906,7 +909,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -926,7 +929,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -955,20 +958,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DB49F4-0D71-45D4-8B24-7BA34D48B26C}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.08203125" customWidth="1"/>
+    <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="57.08203125" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="57" style="1" customWidth="1"/>
+    <col min="6" max="6" width="64.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,17 +982,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -998,14 +1002,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1015,17 +1019,17 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1035,17 +1039,17 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1055,14 +1059,14 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1072,14 +1076,14 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1089,14 +1093,14 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1106,17 +1110,17 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1126,17 +1130,17 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1146,13 +1150,13 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1165,20 +1169,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FE319F-68B5-4879-B9F9-8C755E7FDE1F}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.08203125" customWidth="1"/>
+    <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="57.08203125" customWidth="1"/>
+    <col min="5" max="5" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1218,7 +1222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>

</xml_diff>